<commit_message>
Update CPD and Dataextractor
Update CPD - add AppState
add details to dataextractor
</commit_message>
<xml_diff>
--- a/Wifi bootloader prelim CPD 6.xlsx
+++ b/Wifi bootloader prelim CPD 6.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mernok\DEVPRJ-168 (Booyco HMI)\Software\Booyco-HMI-Utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4210A256-7717-4A1E-967E-6A4F9A20FC93}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AC2BD2-D82E-478F-B548-0231378EA209}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AppState" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="92">
   <si>
     <t>SOF1</t>
   </si>
@@ -292,13 +293,28 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>[26..519]</t>
+  </si>
+  <si>
+    <t>AppState</t>
+  </si>
+  <si>
+    <t>HMI Application</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,8 +381,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +427,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,7 +590,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -568,8 +598,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -644,10 +675,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Explanatory Text" xfId="6" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Linked Cell" xfId="4" builtinId="24"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -964,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF52"/>
+  <dimension ref="A1:AG52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,12 +1029,13 @@
     <col min="16" max="16" width="10" style="6" customWidth="1"/>
     <col min="17" max="18" width="10" style="6" bestFit="1" customWidth="1"/>
     <col min="19" max="27" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="9.140625" style="6"/>
-    <col min="32" max="32" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11" style="6" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="9.140625" style="6"/>
+    <col min="33" max="33" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
@@ -1038,8 +1080,9 @@
       <c r="AD1" s="8"/>
       <c r="AE1" s="8"/>
       <c r="AF1" s="8"/>
-    </row>
-    <row r="2" spans="1:32" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG1" s="8"/>
+    </row>
+    <row r="2" spans="1:33" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>77</v>
       </c>
@@ -1074,8 +1117,9 @@
       <c r="AD2" s="12"/>
       <c r="AE2" s="12"/>
       <c r="AF2" s="12"/>
-    </row>
-    <row r="3" spans="1:32" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AG2" s="12"/>
+    </row>
+    <row r="3" spans="1:33" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>18</v>
       </c>
@@ -1155,21 +1199,24 @@
       <c r="AA3" s="8">
         <v>24</v>
       </c>
-      <c r="AB3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC3" s="8">
+      <c r="AB3" s="8">
+        <v>25</v>
+      </c>
+      <c r="AC3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD3" s="8">
         <v>520</v>
       </c>
-      <c r="AD3" s="8">
+      <c r="AE3" s="8">
         <v>521</v>
       </c>
-      <c r="AE3" s="8">
+      <c r="AF3" s="8">
         <v>522</v>
       </c>
-      <c r="AF3" s="8"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG3" s="8"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1251,23 +1298,26 @@
       <c r="AA4" s="19">
         <v>0</v>
       </c>
-      <c r="AB4" s="19">
+      <c r="AB4" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC4" s="19">
         <v>0</v>
       </c>
-      <c r="AC4" s="19" t="s">
-        <v>4</v>
-      </c>
       <c r="AD4" s="19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE4" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG4" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1349,23 +1399,26 @@
       <c r="AA5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AB5" s="19">
+      <c r="AB5" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC5" s="19">
         <v>0</v>
       </c>
-      <c r="AC5" s="19" t="s">
-        <v>4</v>
-      </c>
       <c r="AD5" s="19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG5" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:32" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>75</v>
       </c>
@@ -1400,8 +1453,9 @@
       <c r="AD6" s="10"/>
       <c r="AE6" s="10"/>
       <c r="AF6" s="10"/>
-    </row>
-    <row r="7" spans="1:32" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AG6" s="10"/>
+    </row>
+    <row r="7" spans="1:33" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1494,8 +1548,9 @@
         <v>522</v>
       </c>
       <c r="AF7" s="8"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG7" s="8"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1528,7 +1583,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1561,7 +1616,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <f>COUNTA(C10:J10)</f>
         <v>8</v>
@@ -1595,7 +1650,7 @@
       </c>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1692,8 +1747,9 @@
       <c r="AF11" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG11" s="31"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1735,7 +1791,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1777,7 +1833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <f>COUNTA(C14:I14)</f>
         <v>7</v>
@@ -1807,7 +1863,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:32" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>76</v>
       </c>
@@ -1842,8 +1898,9 @@
       <c r="AD16" s="10"/>
       <c r="AE16" s="10"/>
       <c r="AF16" s="10"/>
-    </row>
-    <row r="17" spans="1:32" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AG16" s="10"/>
+    </row>
+    <row r="17" spans="1:33" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1936,8 +1993,9 @@
         <v>522</v>
       </c>
       <c r="AF17" s="8"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG17" s="8"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>80</v>
       </c>
@@ -1970,7 +2028,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>24</v>
       </c>
@@ -2003,7 +2061,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>25</v>
       </c>
@@ -2100,8 +2158,9 @@
       <c r="AF20" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG20"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>26</v>
       </c>
@@ -2143,7 +2202,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>27</v>
       </c>
@@ -2182,7 +2241,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>79</v>
       </c>
@@ -2215,7 +2274,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>81</v>
       </c>
@@ -2248,7 +2307,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>82</v>
       </c>
@@ -2281,7 +2340,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>25</v>
       </c>
@@ -2378,8 +2437,9 @@
       <c r="AF27" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG27" s="31"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>26</v>
       </c>
@@ -2421,7 +2481,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>27</v>
       </c>
@@ -2460,7 +2520,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
         <v>79</v>
       </c>
@@ -2493,7 +2553,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <f>COUNTA(C30:I30)</f>
         <v>7</v>
@@ -2523,7 +2583,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <f>COUNTA(C31:I31)</f>
         <v>0</v>
@@ -2553,7 +2613,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:32" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>85</v>
       </c>
@@ -2588,8 +2648,9 @@
       <c r="AD35" s="10"/>
       <c r="AE35" s="10"/>
       <c r="AF35" s="10"/>
-    </row>
-    <row r="36" spans="1:32" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AG35" s="10"/>
+    </row>
+    <row r="36" spans="1:33" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
@@ -2682,8 +2743,9 @@
         <v>522</v>
       </c>
       <c r="AF36" s="8"/>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG36" s="8"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
         <v>80</v>
       </c>
@@ -2716,12 +2778,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="2">
-        <f t="shared" ref="B38:B42" si="3">COUNTA(C38:I38)</f>
+        <f t="shared" ref="B38" si="3">COUNTA(C38:I38)</f>
         <v>7</v>
       </c>
       <c r="C38" s="15" t="s">
@@ -2748,8 +2810,9 @@
       <c r="J38" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG38" s="30"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>25</v>
       </c>
@@ -2846,8 +2909,9 @@
       <c r="AF39" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG39" s="31"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>26</v>
       </c>
@@ -2888,13 +2952,14 @@
       <c r="M40" s="18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG40" s="30"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>27</v>
       </c>
       <c r="B41" s="2">
-        <f t="shared" ref="B41:B45" si="4">COUNTA(C41:I41)</f>
+        <f t="shared" ref="B41:B42" si="4">COUNTA(C41:I41)</f>
         <v>7</v>
       </c>
       <c r="C41" s="15" t="s">
@@ -2927,8 +2992,9 @@
       <c r="L41" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG41" s="30"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>79</v>
       </c>
@@ -2960,8 +3026,12 @@
       <c r="J42" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG42" s="30"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AG43" s="30"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>81</v>
       </c>
@@ -2993,8 +3063,9 @@
       <c r="J44" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG44" s="30"/>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>82</v>
       </c>
@@ -3026,8 +3097,9 @@
       <c r="J45" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG45" s="30"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>25</v>
       </c>
@@ -3124,8 +3196,9 @@
       <c r="AF46" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG46" s="31"/>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>26</v>
       </c>
@@ -3166,8 +3239,9 @@
       <c r="M47" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG47" s="30"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>27</v>
       </c>
@@ -3303,7 +3377,50 @@
   <mergeCells count="1">
     <mergeCell ref="F1:S1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AB5" location="AppState!A1" display="AppState" xr:uid="{DA24C2B6-0CA6-4180-9D9E-2B288D3DE0BE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E141646D-FDCF-48ED-8D52-2ED47270FBDB}">
+  <dimension ref="A2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>